<commit_message>
comparador v8 (Creación de plantillas y comparación de nombres)
</commit_message>
<xml_diff>
--- a/dist/02_150125.xlsx
+++ b/dist/02_150125.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\EXCEL PRUEBA COMPARADOR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\pyAlhambra\pyAlhambra\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C035E7-D101-4701-8063-83A5A25C7095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183B17EC-807E-4755-85FD-543ADE72EF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13560" yWindow="0" windowWidth="13545" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40596" yWindow="6048" windowWidth="21600" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="루밍" sheetId="9" r:id="rId1"/>
@@ -952,9 +952,6 @@
     <t>PASSPORT</t>
   </si>
   <si>
-    <t>YU/HYANGSUK</t>
-  </si>
-  <si>
     <t>M067G5479</t>
   </si>
   <si>
@@ -1076,6 +1073,9 @@
   </si>
   <si>
     <t>M16135181</t>
+  </si>
+  <si>
+    <t>YU/HYANGSUKE</t>
   </si>
 </sst>
 </file>
@@ -2946,19 +2946,19 @@
   </sheetPr>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="2.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1">
+    <row r="1" spans="1:3" ht="15" thickBot="1">
       <c r="A1" s="10"/>
       <c r="B1" s="12" t="s">
         <v>0</v>
@@ -2972,10 +2972,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
@@ -2983,10 +2983,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
@@ -2994,10 +2994,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1" ht="18.75" customHeight="1">
@@ -3005,10 +3005,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
@@ -3016,10 +3016,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
@@ -3027,10 +3027,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
@@ -3038,10 +3038,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
@@ -3049,10 +3049,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
@@ -3060,10 +3060,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
@@ -3071,10 +3071,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
@@ -3082,10 +3082,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="2" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
@@ -3093,10 +3093,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
@@ -3104,10 +3104,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
@@ -3115,10 +3115,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
@@ -3126,10 +3126,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
@@ -3137,10 +3137,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
@@ -3148,10 +3148,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
@@ -3159,10 +3159,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
@@ -3170,10 +3170,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
@@ -3181,10 +3181,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
@@ -3192,10 +3192,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -3210,14 +3210,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3b324d95-18ae-4ef0-925b-59110413f0ec" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e2096bfe-5fc0-4a56-b376-f3fe333f10a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3456,21 +3454,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3b324d95-18ae-4ef0-925b-59110413f0ec" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e2096bfe-5fc0-4a56-b376-f3fe333f10a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4522C266-632E-4F05-B2E0-760837EFC1AA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02FB0FBE-C215-4B1C-9DFA-72CA9D79BEAB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3b324d95-18ae-4ef0-925b-59110413f0ec"/>
-    <ds:schemaRef ds:uri="e2096bfe-5fc0-4a56-b376-f3fe333f10a2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3495,9 +3492,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02FB0FBE-C215-4B1C-9DFA-72CA9D79BEAB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4522C266-632E-4F05-B2E0-760837EFC1AA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3b324d95-18ae-4ef0-925b-59110413f0ec"/>
+    <ds:schemaRef ds:uri="e2096bfe-5fc0-4a56-b376-f3fe333f10a2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>